<commit_message>
edits to flag script
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/test images.xlsx
+++ b/fifty_one/measurements/test images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilbenor/Documents/code projects/msc/counting_research_algorithms/fifty_one/measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1F512F-4153-DA44-A11E-B4F301E7FAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A48D3B-9EB6-7F4F-B633-F9330604FCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="140">
   <si>
     <t>file name</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>height(mm)</t>
+  </si>
+  <si>
+    <t>height(mm)111</t>
   </si>
 </sst>
 </file>
@@ -803,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -833,7 +836,7 @@
     <col min="25" max="25" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -847,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -858,8 +861,11 @@
       <c r="H1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -880,8 +886,12 @@
         <f>CONCATENATE("GX010", TEXT(G2, "0"))</f>
         <v>GX010067_625</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <f>E2-10</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -901,8 +911,12 @@
         <f t="shared" ref="H3:H66" si="0">CONCATENATE("GX010", TEXT(G3, "0"))</f>
         <v>GX010068_666</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="1">E3-10</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -923,8 +937,12 @@
         <f t="shared" si="0"/>
         <v>GX010068_795</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -945,8 +963,12 @@
         <f t="shared" si="0"/>
         <v>GX010069_191</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -967,8 +989,12 @@
         <f t="shared" si="0"/>
         <v>GX010069_796</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -992,8 +1018,12 @@
         <f t="shared" si="0"/>
         <v>GX010071_444</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1017,8 +1047,12 @@
         <f t="shared" si="0"/>
         <v>GX010101_173</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1042,8 +1076,12 @@
         <f t="shared" si="0"/>
         <v>GX010102_1396</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1067,8 +1105,12 @@
         <f t="shared" si="0"/>
         <v>GX010102_165</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -1092,8 +1134,12 @@
         <f t="shared" si="0"/>
         <v>GX010105_816</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1117,8 +1163,12 @@
         <f t="shared" si="0"/>
         <v>GX010128_52</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1142,8 +1192,12 @@
         <f t="shared" si="0"/>
         <v>GX010128_54</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1167,8 +1221,12 @@
         <f t="shared" si="0"/>
         <v>GX010129_454</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1192,8 +1250,12 @@
         <f t="shared" si="0"/>
         <v>GX010139_2020</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1217,8 +1279,12 @@
         <f t="shared" si="0"/>
         <v>GX010144_3581</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1242,8 +1308,12 @@
         <f t="shared" si="0"/>
         <v>GX010145_2273</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1255,7 +1325,7 @@
         <v>24</v>
       </c>
       <c r="E18">
-        <v>530</v>
+        <v>415</v>
       </c>
       <c r="F18" s="1">
         <v>12</v>
@@ -1267,8 +1337,12 @@
         <f t="shared" si="0"/>
         <v>GX010152_378</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1292,8 +1366,12 @@
         <f t="shared" si="0"/>
         <v>GX010154_4137</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1313,8 +1391,12 @@
         <f t="shared" si="0"/>
         <v>GX010154_933</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -1334,8 +1416,12 @@
         <f t="shared" si="0"/>
         <v>GX010155_1170</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -1361,8 +1447,12 @@
         <f t="shared" si="0"/>
         <v>GX010155_219</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1382,8 +1472,12 @@
         <f t="shared" si="0"/>
         <v>GX010156_629</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -1409,8 +1503,12 @@
         <f t="shared" si="0"/>
         <v>GX010156_662</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1430,8 +1528,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_2240</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1451,8 +1553,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_2259</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1472,8 +1578,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_2554</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1499,8 +1609,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_2582</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1526,8 +1640,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_2665</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1547,8 +1665,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_4575</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -1574,8 +1696,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_4691</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1601,8 +1727,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_5053</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1622,8 +1752,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_5205</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1649,8 +1783,12 @@
         <f t="shared" si="0"/>
         <v>GX010157_883</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1674,8 +1812,12 @@
         <f t="shared" si="0"/>
         <v>GX010158_1158</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1695,8 +1837,12 @@
         <f t="shared" si="0"/>
         <v>GX010161_2267</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1716,8 +1862,12 @@
         <f t="shared" si="0"/>
         <v>GX010161_676</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1743,8 +1893,12 @@
         <f t="shared" si="0"/>
         <v>GX010161_9576</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1770,8 +1924,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_2037</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1791,8 +1949,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_2230</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1812,8 +1974,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_2433</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1839,8 +2005,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_2604</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1866,8 +2036,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_3958</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1887,8 +2061,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_4175</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1914,8 +2092,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_687</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1941,8 +2123,12 @@
         <f t="shared" si="0"/>
         <v>GX010162_927</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1968,8 +2154,12 @@
         <f t="shared" si="0"/>
         <v>GX010163_798</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -1989,8 +2179,12 @@
         <f t="shared" si="0"/>
         <v>GX010163_864</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2010,8 +2204,12 @@
         <f t="shared" si="0"/>
         <v>GX010169_1249</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2037,8 +2235,12 @@
         <f t="shared" si="0"/>
         <v>GX010170_1546</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2058,8 +2260,12 @@
         <f t="shared" si="0"/>
         <v>GX010171_1483</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -2079,8 +2285,12 @@
         <f t="shared" si="0"/>
         <v>GX010173_922</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2104,8 +2314,12 @@
         <f t="shared" si="0"/>
         <v>GX010174_1236</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -2125,8 +2339,12 @@
         <f t="shared" si="0"/>
         <v>GX010174_2266</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -2150,8 +2368,12 @@
         <f t="shared" si="0"/>
         <v>GX010174_2291</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2171,8 +2393,12 @@
         <f t="shared" si="0"/>
         <v>GX010174_790</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -2196,8 +2422,12 @@
         <f t="shared" si="0"/>
         <v>GX010175_2644</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2217,8 +2447,12 @@
         <f t="shared" si="0"/>
         <v>GX010175_3372</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2238,8 +2472,12 @@
         <f t="shared" si="0"/>
         <v>GX010175_852</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2263,8 +2501,12 @@
         <f t="shared" si="0"/>
         <v>GX010175_865</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -2288,8 +2530,12 @@
         <f t="shared" si="0"/>
         <v>GX010176_1622</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -2309,8 +2555,12 @@
         <f t="shared" si="0"/>
         <v>GX010177_3047</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>58</v>
       </c>
@@ -2334,8 +2584,12 @@
         <f t="shared" si="0"/>
         <v>GX010177_454</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2359,8 +2613,12 @@
         <f t="shared" si="0"/>
         <v>GX010178_2118</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64">
+        <f t="shared" si="1"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -2380,8 +2638,12 @@
         <f t="shared" si="0"/>
         <v>GX010178_2258</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65">
+        <f t="shared" si="1"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -2401,8 +2663,12 @@
         <f t="shared" si="0"/>
         <v>GX010178_3604</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66">
+        <f t="shared" si="1"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -2423,11 +2689,15 @@
         <v>63</v>
       </c>
       <c r="H67" s="4" t="str">
-        <f t="shared" ref="H67:H115" si="1">CONCATENATE("GX010", TEXT(G67, "0"))</f>
+        <f t="shared" ref="H67:H115" si="2">CONCATENATE("GX010", TEXT(G67, "0"))</f>
         <v>GX010178_3987</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67">
+        <f t="shared" ref="I67:I115" si="3">E67-10</f>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>62</v>
       </c>
@@ -2448,11 +2718,15 @@
         <v>65</v>
       </c>
       <c r="H68" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010179_1697</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>62</v>
       </c>
@@ -2473,11 +2747,15 @@
         <v>66</v>
       </c>
       <c r="H69" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010179_3535</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>62</v>
       </c>
@@ -2494,11 +2772,15 @@
         <v>93</v>
       </c>
       <c r="H70" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010179_3927</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -2519,11 +2801,15 @@
         <v>67</v>
       </c>
       <c r="H71" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010179_3942</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>62</v>
       </c>
@@ -2544,11 +2830,15 @@
         <v>64</v>
       </c>
       <c r="H72" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010179_869</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -2569,11 +2859,15 @@
         <v>22</v>
       </c>
       <c r="H73" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010180_1563</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>62</v>
       </c>
@@ -2594,11 +2888,15 @@
         <v>24</v>
       </c>
       <c r="H74" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010180_1788</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>62</v>
       </c>
@@ -2619,11 +2917,15 @@
         <v>25</v>
       </c>
       <c r="H75" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010181_1542</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>62</v>
       </c>
@@ -2644,11 +2946,15 @@
         <v>27</v>
       </c>
       <c r="H76" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010182_1468</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>62</v>
       </c>
@@ -2669,11 +2975,15 @@
         <v>28</v>
       </c>
       <c r="H77" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010182_1822</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>62</v>
       </c>
@@ -2694,11 +3004,15 @@
         <v>26</v>
       </c>
       <c r="H78" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010182_894</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>62</v>
       </c>
@@ -2719,11 +3033,15 @@
         <v>30</v>
       </c>
       <c r="H79" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010183_1633</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>62</v>
       </c>
@@ -2744,11 +3062,15 @@
         <v>31</v>
       </c>
       <c r="H80" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010183_2852</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>62</v>
       </c>
@@ -2769,11 +3091,15 @@
         <v>29</v>
       </c>
       <c r="H81" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010183_685</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>62</v>
       </c>
@@ -2794,11 +3120,15 @@
         <v>33</v>
       </c>
       <c r="H82" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010184_1969</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>62</v>
       </c>
@@ -2819,11 +3149,15 @@
         <v>32</v>
       </c>
       <c r="H83" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010184_890</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83">
+        <f t="shared" si="3"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>68</v>
       </c>
@@ -2844,11 +3178,15 @@
         <v>104</v>
       </c>
       <c r="H84" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010073_1014</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -2869,11 +3207,15 @@
         <v>105</v>
       </c>
       <c r="H85" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010073_695</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I85">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>68</v>
       </c>
@@ -2894,11 +3236,15 @@
         <v>106</v>
       </c>
       <c r="H86" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010077_237</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>69</v>
       </c>
@@ -2919,11 +3265,15 @@
         <v>107</v>
       </c>
       <c r="H87" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010080_2283</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>69</v>
       </c>
@@ -2944,11 +3294,15 @@
         <v>108</v>
       </c>
       <c r="H88" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010080_2640</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>69</v>
       </c>
@@ -2969,11 +3323,15 @@
         <v>109</v>
       </c>
       <c r="H89" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010080_2954</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>69</v>
       </c>
@@ -2994,11 +3352,15 @@
         <v>110</v>
       </c>
       <c r="H90" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010080_3366</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I90">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>69</v>
       </c>
@@ -3019,11 +3381,15 @@
         <v>111</v>
       </c>
       <c r="H91" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010080_3392</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>69</v>
       </c>
@@ -3044,11 +3410,15 @@
         <v>112</v>
       </c>
       <c r="H92" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010082_1070</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I92">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>69</v>
       </c>
@@ -3069,11 +3439,15 @@
         <v>113</v>
       </c>
       <c r="H93" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010082_3137</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I93">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>69</v>
       </c>
@@ -3094,11 +3468,15 @@
         <v>114</v>
       </c>
       <c r="H94" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010082_59</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>69</v>
       </c>
@@ -3119,11 +3497,15 @@
         <v>115</v>
       </c>
       <c r="H95" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010082_796</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I95">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>69</v>
       </c>
@@ -3144,11 +3526,15 @@
         <v>116</v>
       </c>
       <c r="H96" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010084_1748</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I96">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>69</v>
       </c>
@@ -3169,11 +3555,15 @@
         <v>131</v>
       </c>
       <c r="H97" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010084_344</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>69</v>
       </c>
@@ -3194,11 +3584,15 @@
         <v>117</v>
       </c>
       <c r="H98" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010085_3610</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>69</v>
       </c>
@@ -3219,11 +3613,15 @@
         <v>118</v>
       </c>
       <c r="H99" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010085_3738</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I99">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>69</v>
       </c>
@@ -3244,11 +3642,15 @@
         <v>119</v>
       </c>
       <c r="H100" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010088_3712</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I100">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>69</v>
       </c>
@@ -3269,11 +3671,15 @@
         <v>120</v>
       </c>
       <c r="H101" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010088_4364</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I101">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>69</v>
       </c>
@@ -3294,11 +3700,15 @@
         <v>121</v>
       </c>
       <c r="H102" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010089_236</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I102">
+        <f t="shared" si="3"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>69</v>
       </c>
@@ -3319,11 +3729,15 @@
         <v>122</v>
       </c>
       <c r="H103" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010090_1852</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I103">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>69</v>
       </c>
@@ -3344,11 +3758,15 @@
         <v>123</v>
       </c>
       <c r="H104" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010091_149</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I104">
+        <f t="shared" si="3"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>70</v>
       </c>
@@ -3369,11 +3787,15 @@
         <v>124</v>
       </c>
       <c r="H105" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010094_1258</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I105">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>70</v>
       </c>
@@ -3394,11 +3816,15 @@
         <v>125</v>
       </c>
       <c r="H106" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010094_129</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I106">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>70</v>
       </c>
@@ -3419,11 +3845,15 @@
         <v>126</v>
       </c>
       <c r="H107" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010094_2312</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I107">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>70</v>
       </c>
@@ -3444,11 +3874,15 @@
         <v>133</v>
       </c>
       <c r="H108" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010094_430</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I108">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -3469,11 +3903,15 @@
         <v>127</v>
       </c>
       <c r="H109" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010096_1571</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I109">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>70</v>
       </c>
@@ -3494,11 +3932,15 @@
         <v>128</v>
       </c>
       <c r="H110" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010097_1080</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I110">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>70</v>
       </c>
@@ -3519,11 +3961,15 @@
         <v>129</v>
       </c>
       <c r="H111" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010097_1651</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I111">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>70</v>
       </c>
@@ -3544,11 +3990,15 @@
         <v>134</v>
       </c>
       <c r="H112" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010097_1870</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I112">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>70</v>
       </c>
@@ -3569,11 +4019,15 @@
         <v>130</v>
       </c>
       <c r="H113" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010097_528</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I113">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>69</v>
       </c>
@@ -3587,11 +4041,15 @@
         <v>132</v>
       </c>
       <c r="H114" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010088_2904</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I114">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>69</v>
       </c>
@@ -3605,8 +4063,12 @@
         <v>136</v>
       </c>
       <c r="H115" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GX010084_2291</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="3"/>
+        <v>640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>